<commit_message>
adds dtd and assets, renames files, validates
</commit_message>
<xml_diff>
--- a/original/dataFromICL.xlsx
+++ b/original/dataFromICL.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\d_drive\bob\projects\fairspec\henry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hansonr\git\FAIRSpec-EAD\original\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="C01" sheetId="2" r:id="rId1"/>
@@ -142,9 +142,6 @@
     <t>InChIKey=IZQDYJOODYXWEN-OYVNLZQHNA-N</t>
   </si>
   <si>
-    <t>&lt;/note&gt;</t>
-  </si>
-  <si>
     <t>13C.zip</t>
   </si>
   <si>
@@ -190,18 +187,6 @@
     <t>Chemdraw connection file</t>
   </si>
   <si>
-    <t>&lt;note type="type"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;/note&gt;&lt;note type="filename"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;/note&gt;&lt;note type="size"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;/note&gt;&lt;note type="mime-type"&gt;</t>
-  </si>
-  <si>
     <t>https://data.hpc.imperial.ac.uk/resolve/?doi=6681&amp;file=1</t>
   </si>
   <si>
@@ -214,25 +199,40 @@
     <t>&lt;/daodesc&gt;&lt;/dao&gt;</t>
   </si>
   <si>
-    <t>&lt;note type="chem-name"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;/note&gt;&lt;note type="chem-inchi"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;/note&gt;&lt;note type="chem-inchikey"&gt;</t>
-  </si>
-  <si>
     <t>dataset</t>
   </si>
   <si>
     <t>model cdx</t>
   </si>
   <si>
-    <t>&lt;dao type="nmr" class="#CLASS#" href="#HREF#"&gt;&lt;daodesc&gt;</t>
-  </si>
-  <si>
-    <t>&lt;dao type="compound" class="compound" href="#"&gt;&lt;daodesc&gt;</t>
+    <t>&lt;note type="type"&gt;&lt;p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/p&gt;&lt;/note&gt;&lt;note type="filename"&gt;&lt;p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/p&gt;&lt;/note&gt;&lt;note type="mime-type"&gt;&lt;p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/p&gt;&lt;/note&gt;&lt;note type="size"&gt;&lt;p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/p&gt;&lt;/note&gt;</t>
+  </si>
+  <si>
+    <t>&lt;dao role="nmr:#CLASS#" href="#HREF#"&gt;&lt;daodesc&gt;</t>
+  </si>
+  <si>
+    <t>&lt;note type="chem-name"&gt;&lt;p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchi"&gt;&lt;p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchikey"&gt;&lt;p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;did&gt;&lt;note&gt;&lt;p&gt;compound&lt;/p&gt;&lt;/note&gt;&lt;/did&gt;&lt;dao role="compound" href="#"&gt;&lt;daodesc&gt;</t>
   </si>
 </sst>
 </file>
@@ -1073,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1228,79 +1228,79 @@
         <v>70</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="str">
         <f>SUBSTITUTE($A$12,"#",SUBSTITUTE(B1,"&amp;","&amp;amp;"))&amp;$B$12&amp;A1&amp;$C$12&amp;C1&amp;$D$12&amp;D1&amp;$E$12&amp;$F$12&amp;$G$12</f>
-        <v>&lt;dao type="compound" class="compound" href="https://doi.org/10.14469/hpc/6681"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;6-propyltetrahydro-2H-pyran-2-ol&lt;/note&gt;&lt;note type="chem-inchi"&gt;InChI=1S/C8H16O2/c1-2-4-7-5-3-6-8(9)10-7/h7-9H,2-6H2,1H3/t7-,8+/m0/s1&lt;/note&gt;&lt;note type="chem-inchikey"&gt;InChIKey=MNGKKXNULWENEQ-JGVFFNPUNA-N&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
+        <v>&lt;did&gt;&lt;note&gt;&lt;p&gt;compound&lt;/p&gt;&lt;/note&gt;&lt;/did&gt;&lt;dao role="compound" href="https://doi.org/10.14469/hpc/6681"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;&lt;p&gt;6-propyltetrahydro-2H-pyran-2-ol&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchi"&gt;&lt;p&gt;InChI=1S/C8H16O2/c1-2-4-7-5-3-6-8(9)10-7/h7-9H,2-6H2,1H3/t7-,8+/m0/s1&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchikey"&gt;&lt;p&gt;InChIKey=MNGKKXNULWENEQ-JGVFFNPUNA-N&lt;/p&gt;&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="str">
         <f t="shared" ref="A15:A23" si="0">SUBSTITUTE($A$12,"#",SUBSTITUTE(B2,"&amp;","&amp;amp;"))&amp;$B$12&amp;A2&amp;$C$12&amp;C2&amp;$D$12&amp;D2&amp;$E$12&amp;$F$12&amp;$G$12</f>
-        <v>&lt;dao type="compound" class="compound" href="https://doi.org/10.14469/hpc/6682"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;6-methyltetrahydro-2H-pyran-2-ol&lt;/note&gt;&lt;note type="chem-inchi"&gt;InChI=1S/C6H12O2/c1-5-3-2-4-6(7)8-5/h5-7H,2-4H2,1H3/t5-,6+/m0/s1&lt;/note&gt;&lt;note type="chem-inchikey"&gt;InChIKey=XCNWVNNDBZRDEA-NTSWFWBYNA-N&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
+        <v>&lt;did&gt;&lt;note&gt;&lt;p&gt;compound&lt;/p&gt;&lt;/note&gt;&lt;/did&gt;&lt;dao role="compound" href="https://doi.org/10.14469/hpc/6682"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;&lt;p&gt;6-methyltetrahydro-2H-pyran-2-ol&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchi"&gt;&lt;p&gt;InChI=1S/C6H12O2/c1-5-3-2-4-6(7)8-5/h5-7H,2-4H2,1H3/t5-,6+/m0/s1&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchikey"&gt;&lt;p&gt;InChIKey=XCNWVNNDBZRDEA-NTSWFWBYNA-N&lt;/p&gt;&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;dao type="compound" class="compound" href="https://doi.org/10.14469/hpc/6683"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;tetrahydro-2H-pyran-2-ol&lt;/note&gt;&lt;note type="chem-inchi"&gt;InChI=1S/C5H10O2/c6-5-3-1-2-4-7-5/h5-6H,1-4H2/t5-/m0/s1&lt;/note&gt;&lt;note type="chem-inchikey"&gt;InChIKey=CELWCAITJAEQNL-YFKPBYRVNA-N&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
+        <v>&lt;did&gt;&lt;note&gt;&lt;p&gt;compound&lt;/p&gt;&lt;/note&gt;&lt;/did&gt;&lt;dao role="compound" href="https://doi.org/10.14469/hpc/6683"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;&lt;p&gt;tetrahydro-2H-pyran-2-ol&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchi"&gt;&lt;p&gt;InChI=1S/C5H10O2/c6-5-3-1-2-4-7-5/h5-6H,1-4H2/t5-/m0/s1&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchikey"&gt;&lt;p&gt;InChIKey=CELWCAITJAEQNL-YFKPBYRVNA-N&lt;/p&gt;&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;dao type="compound" class="compound" href="https://doi.org/10.14469/hpc/6684"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;6-pentyltetrahydro-2H-pyran-2-ol&lt;/note&gt;&lt;note type="chem-inchi"&gt;InChI=1S/C10H20O2/c1-2-3-4-6-9-7-5-8-10(11)12-9/h9-11H,2-8H2,1H3/t9-,10+/m0/s1&lt;/note&gt;&lt;note type="chem-inchikey"&gt;InChIKey=MQEDUMDVRONSJZ-VHSXEESVNA-N&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
+        <v>&lt;did&gt;&lt;note&gt;&lt;p&gt;compound&lt;/p&gt;&lt;/note&gt;&lt;/did&gt;&lt;dao role="compound" href="https://doi.org/10.14469/hpc/6684"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;&lt;p&gt;6-pentyltetrahydro-2H-pyran-2-ol&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchi"&gt;&lt;p&gt;InChI=1S/C10H20O2/c1-2-3-4-6-9-7-5-8-10(11)12-9/h9-11H,2-8H2,1H3/t9-,10+/m0/s1&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchikey"&gt;&lt;p&gt;InChIKey=MQEDUMDVRONSJZ-VHSXEESVNA-N&lt;/p&gt;&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;dao type="compound" class="compound" href="https://doi.org/10.14469/hpc/6685"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;(R)-hexane-1,5-diyl dibenzoate&lt;/note&gt;&lt;note type="chem-inchi"&gt;InChI=1S/C20H22O4/c1-16(24-20(22)18-13-6-3-7-14-18)10-8-9-15-23-19(21)17-11-4-2-5-12-17/h2-7,11-14,16H,8-10,15H2,1H3/t16-/m1/s1&lt;/note&gt;&lt;note type="chem-inchikey"&gt;InChIKey=ALCRVMODCYBKAK-MRXNPFEDNA-N&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
+        <v>&lt;did&gt;&lt;note&gt;&lt;p&gt;compound&lt;/p&gt;&lt;/note&gt;&lt;/did&gt;&lt;dao role="compound" href="https://doi.org/10.14469/hpc/6685"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;&lt;p&gt;(R)-hexane-1,5-diyl dibenzoate&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchi"&gt;&lt;p&gt;InChI=1S/C20H22O4/c1-16(24-20(22)18-13-6-3-7-14-18)10-8-9-15-23-19(21)17-11-4-2-5-12-17/h2-7,11-14,16H,8-10,15H2,1H3/t16-/m1/s1&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchikey"&gt;&lt;p&gt;InChIKey=ALCRVMODCYBKAK-MRXNPFEDNA-N&lt;/p&gt;&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;dao type="compound" class="compound" href="https://doi.org/10.14469/hpc/6686"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;(R)-octane-1,5-diyl dibenzoate&lt;/note&gt;&lt;note type="chem-inchi"&gt;InChI=1S/C22H26O4/c1-2-11-20(26-22(24)19-14-7-4-8-15-19)16-9-10-17-25-21(23)18-12-5-3-6-13-18/h3-8,12-15,20H,2,9-11,16-17H2,1H3/t20-/m1/s1&lt;/note&gt;&lt;note type="chem-inchikey"&gt;InChIKey=DWNNCWYUUFBKIX-HXUWFJFHNA-N&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
+        <v>&lt;did&gt;&lt;note&gt;&lt;p&gt;compound&lt;/p&gt;&lt;/note&gt;&lt;/did&gt;&lt;dao role="compound" href="https://doi.org/10.14469/hpc/6686"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;&lt;p&gt;(R)-octane-1,5-diyl dibenzoate&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchi"&gt;&lt;p&gt;InChI=1S/C22H26O4/c1-2-11-20(26-22(24)19-14-7-4-8-15-19)16-9-10-17-25-21(23)18-12-5-3-6-13-18/h3-8,12-15,20H,2,9-11,16-17H2,1H3/t20-/m1/s1&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchikey"&gt;&lt;p&gt;InChIKey=DWNNCWYUUFBKIX-HXUWFJFHNA-N&lt;/p&gt;&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;dao type="compound" class="compound" href="https://doi.org/10.14469/hpc/6687"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;(R)-decane-1,5-diyl dibenzoate&lt;/note&gt;&lt;note type="chem-inchi"&gt;InChI=1S/C24H30O4/c1-2-3-6-17-22(28-24(26)21-15-9-5-10-16-21)18-11-12-19-27-23(25)20-13-7-4-8-14-20/h4-5,7-10,13-16,22H,2-3,6,11-12,17-19H2,1H3/t22-/m1/s1&lt;/note&gt;&lt;note type="chem-inchikey"&gt;InChIKey=VFEFIKPQIOEYNR-JOCHJYFZNA-N&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
+        <v>&lt;did&gt;&lt;note&gt;&lt;p&gt;compound&lt;/p&gt;&lt;/note&gt;&lt;/did&gt;&lt;dao role="compound" href="https://doi.org/10.14469/hpc/6687"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;&lt;p&gt;(R)-decane-1,5-diyl dibenzoate&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchi"&gt;&lt;p&gt;InChI=1S/C24H30O4/c1-2-3-6-17-22(28-24(26)21-15-9-5-10-16-21)18-11-12-19-27-23(25)20-13-7-4-8-14-20/h4-5,7-10,13-16,22H,2-3,6,11-12,17-19H2,1H3/t22-/m1/s1&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchikey"&gt;&lt;p&gt;InChIKey=VFEFIKPQIOEYNR-JOCHJYFZNA-N&lt;/p&gt;&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;dao type="compound" class="compound" href="https://doi.org/10.14469/hpc/6688"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;(R,E)-5-hydroxyhexanal oxime&lt;/note&gt;&lt;note type="chem-inchi"&gt;InChI=1S/C6H13NO2/c1-6(8)4-2-3-5-7-9/h5-6,8-9H,2-4H2,1H3/b7-5+/t6-/m1/s1&lt;/note&gt;&lt;note type="chem-inchikey"&gt;InChIKey=LUZLJFZRMFXZEE-LUFONEFENA-N&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
+        <v>&lt;did&gt;&lt;note&gt;&lt;p&gt;compound&lt;/p&gt;&lt;/note&gt;&lt;/did&gt;&lt;dao role="compound" href="https://doi.org/10.14469/hpc/6688"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;&lt;p&gt;(R,E)-5-hydroxyhexanal oxime&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchi"&gt;&lt;p&gt;InChI=1S/C6H13NO2/c1-6(8)4-2-3-5-7-9/h5-6,8-9H,2-4H2,1H3/b7-5+/t6-/m1/s1&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchikey"&gt;&lt;p&gt;InChIKey=LUZLJFZRMFXZEE-LUFONEFENA-N&lt;/p&gt;&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;dao type="compound" class="compound" href="https://doi.org/10.14469/hpc/6689"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;(R,E)-5-hydroxyoctanal oxime&lt;/note&gt;&lt;note type="chem-inchi"&gt;InChI=1S/C8H17NO2/c1-2-5-8(10)6-3-4-7-9-11/h7-8,10-11H,2-6H2,1H3/b9-7+/t8-/m1/s1&lt;/note&gt;&lt;note type="chem-inchikey"&gt;InChIKey=SVPUVGPIADWQEK-KGOFQHAKNA-N&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
+        <v>&lt;did&gt;&lt;note&gt;&lt;p&gt;compound&lt;/p&gt;&lt;/note&gt;&lt;/did&gt;&lt;dao role="compound" href="https://doi.org/10.14469/hpc/6689"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;&lt;p&gt;(R,E)-5-hydroxyoctanal oxime&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchi"&gt;&lt;p&gt;InChI=1S/C8H17NO2/c1-2-5-8(10)6-3-4-7-9-11/h7-8,10-11H,2-6H2,1H3/b9-7+/t8-/m1/s1&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchikey"&gt;&lt;p&gt;InChIKey=SVPUVGPIADWQEK-KGOFQHAKNA-N&lt;/p&gt;&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;dao type="compound" class="compound" href="https://doi.org/10.14469/hpc/6690"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;(R)-5-hydroxydecanal oxime&lt;/note&gt;&lt;note type="chem-inchi"&gt;InChI=1S/C10H21NO2/c1-2-3-4-7-10(12)8-5-6-9-11-13/h9-10,12-13H,2-8H2,1H3/b11-9+/t10-/m1/s1&lt;/note&gt;&lt;note type="chem-inchikey"&gt;InChIKey=IZQDYJOODYXWEN-OYVNLZQHNA-N&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
+        <v>&lt;did&gt;&lt;note&gt;&lt;p&gt;compound&lt;/p&gt;&lt;/note&gt;&lt;/did&gt;&lt;dao role="compound" href="https://doi.org/10.14469/hpc/6690"&gt;&lt;daodesc&gt;&lt;note type="chem-name"&gt;&lt;p&gt;(R)-5-hydroxydecanal oxime&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchi"&gt;&lt;p&gt;InChI=1S/C10H21NO2/c1-2-3-4-7-10(12)8-5-6-9-11-13/h9-10,12-13H,2-8H2,1H3/b11-9+/t10-/m1/s1&lt;/p&gt;&lt;/note&gt;&lt;note type="chem-inchikey"&gt;&lt;p&gt;InChIKey=IZQDYJOODYXWEN-OYVNLZQHNA-N&lt;/p&gt;&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
       </c>
     </row>
   </sheetData>
@@ -1312,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1325,132 +1325,132 @@
   <sheetData>
     <row r="1" spans="1:18" ht="11.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" t="s">
-        <v>44</v>
-      </c>
       <c r="F1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
       <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" t="s">
-        <v>44</v>
-      </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
         <v>47</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>48</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>49</v>
       </c>
-      <c r="E3" t="s">
-        <v>50</v>
-      </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>52</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" t="s">
         <v>54</v>
       </c>
-      <c r="E4" t="s">
-        <v>55</v>
-      </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="R4" s="3"/>
     </row>
     <row r="7" spans="1:18" ht="12" customHeight="1"/>
     <row r="12" spans="1:18" s="4" customFormat="1">
       <c r="A12" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="R12" s="5"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="str">
         <f>SUBSTITUTE(SUBSTITUTE($A$12,"#HREF#",SUBSTITUTE(A1,"&amp;","&amp;amp;")), "#CLASS#",F1)&amp;$B$12&amp;E1&amp;$C$12&amp;B1&amp;$D$12&amp;C1&amp;$E$12&amp;D1&amp;$F$12&amp;$J$12</f>
-        <v>&lt;dao type="nmr" class="dataset" href="https://data.hpc.imperial.ac.uk/resolve/?doi=6681&amp;amp;file=1"&gt;&lt;daodesc&gt;&lt;note type="type"&gt;Bruker Dataset&lt;/note&gt;&lt;note type="filename"&gt;13C.zip&lt;/note&gt;&lt;note type="size"&gt;966KB&lt;/note&gt;&lt;note type="mime-type"&gt;application/zip&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
+        <v>&lt;dao role="nmr:dataset" href="https://data.hpc.imperial.ac.uk/resolve/?doi=6681&amp;amp;file=1"&gt;&lt;daodesc&gt;&lt;note type="type"&gt;&lt;p&gt;Bruker Dataset&lt;/p&gt;&lt;/note&gt;&lt;note type="filename"&gt;&lt;p&gt;13C.zip&lt;/p&gt;&lt;/note&gt;&lt;note type="size"&gt;&lt;p&gt;966KB&lt;/p&gt;&lt;/note&gt;&lt;note type="mime-type"&gt;&lt;p&gt;application/zip&lt;/p&gt;&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="str">
         <f>SUBSTITUTE(SUBSTITUTE($A$12,"#HREF#",SUBSTITUTE(A2,"&amp;","&amp;amp;")), "#CLASS#",F2)&amp;$B$12&amp;E2&amp;$C$12&amp;B2&amp;$D$12&amp;C2&amp;$E$12&amp;D2&amp;$F$12&amp;$J$12</f>
-        <v>&lt;dao type="nmr" class="dataset" href="https://data.hpc.imperial.ac.uk/resolve/?doi=6681&amp;amp;file=2"&gt;&lt;daodesc&gt;&lt;note type="type"&gt;Bruker Dataset&lt;/note&gt;&lt;note type="filename"&gt;1H.zip&lt;/note&gt;&lt;note type="size"&gt;684KB&lt;/note&gt;&lt;note type="mime-type"&gt;application/zip&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
+        <v>&lt;dao role="nmr:dataset" href="https://data.hpc.imperial.ac.uk/resolve/?doi=6681&amp;amp;file=2"&gt;&lt;daodesc&gt;&lt;note type="type"&gt;&lt;p&gt;Bruker Dataset&lt;/p&gt;&lt;/note&gt;&lt;note type="filename"&gt;&lt;p&gt;1H.zip&lt;/p&gt;&lt;/note&gt;&lt;note type="size"&gt;&lt;p&gt;684KB&lt;/p&gt;&lt;/note&gt;&lt;note type="mime-type"&gt;&lt;p&gt;application/zip&lt;/p&gt;&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="str">
         <f>SUBSTITUTE(SUBSTITUTE($A$12,"#HREF#",SUBSTITUTE(A3,"&amp;","&amp;amp;")), "#CLASS#",F3)&amp;$B$12&amp;E3&amp;$C$12&amp;B3&amp;$D$12&amp;C3&amp;$E$12&amp;D3&amp;$F$12&amp;$J$12</f>
-        <v>&lt;dao type="nmr" class="dataset" href="https://data.hpc.imperial.ac.uk/resolve/?doi=6681&amp;amp;file=3"&gt;&lt;daodesc&gt;&lt;note type="type"&gt;Mestranova Dataset&lt;/note&gt;&lt;note type="filename"&gt;lactol 1c.mnova&lt;/note&gt;&lt;note type="size"&gt;705KB&lt;/note&gt;&lt;note type="mime-type"&gt;chemical/x-mnova&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
+        <v>&lt;dao role="nmr:dataset" href="https://data.hpc.imperial.ac.uk/resolve/?doi=6681&amp;amp;file=3"&gt;&lt;daodesc&gt;&lt;note type="type"&gt;&lt;p&gt;Mestranova Dataset&lt;/p&gt;&lt;/note&gt;&lt;note type="filename"&gt;&lt;p&gt;lactol 1c.mnova&lt;/p&gt;&lt;/note&gt;&lt;note type="size"&gt;&lt;p&gt;705KB&lt;/p&gt;&lt;/note&gt;&lt;note type="mime-type"&gt;&lt;p&gt;chemical/x-mnova&lt;/p&gt;&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="str">
         <f>SUBSTITUTE(SUBSTITUTE($A$12,"#HREF#",SUBSTITUTE(A4,"&amp;","&amp;amp;")), "#CLASS#",F4)&amp;$B$12&amp;E4&amp;$C$12&amp;B4&amp;$D$12&amp;C4&amp;$E$12&amp;D4&amp;$F$12&amp;$J$12</f>
-        <v>&lt;dao type="nmr" class="model cdx" href="https://data.hpc.imperial.ac.uk/resolve/?doi=6681&amp;amp;file=4"&gt;&lt;daodesc&gt;&lt;note type="type"&gt;Chemdraw connection file&lt;/note&gt;&lt;note type="filename"&gt;6-propyltetrahydro-2H-pyran-2-ol.cdxml&lt;/note&gt;&lt;note type="size"&gt;5KB&lt;/note&gt;&lt;note type="mime-type"&gt;chemical/x-cdxml&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
+        <v>&lt;dao role="nmr:model cdx" href="https://data.hpc.imperial.ac.uk/resolve/?doi=6681&amp;amp;file=4"&gt;&lt;daodesc&gt;&lt;note type="type"&gt;&lt;p&gt;Chemdraw connection file&lt;/p&gt;&lt;/note&gt;&lt;note type="filename"&gt;&lt;p&gt;6-propyltetrahydro-2H-pyran-2-ol.cdxml&lt;/p&gt;&lt;/note&gt;&lt;note type="size"&gt;&lt;p&gt;5KB&lt;/p&gt;&lt;/note&gt;&lt;note type="mime-type"&gt;&lt;p&gt;chemical/x-cdxml&lt;/p&gt;&lt;/note&gt;&lt;/daodesc&gt;&lt;/dao&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>